<commit_message>
feat(data): update metadata file
</commit_message>
<xml_diff>
--- a/data/pdf/metadata_pdf_file.xlsx
+++ b/data/pdf/metadata_pdf_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clovi\Documents\WIKIT\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\Code\wikit\bench-chunknorris-acl2025\data\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D93F00C1-51E5-4017-9FCB-6EDDFF4B5D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ACBBE4-76AB-4438-B5F8-4338B0A4D9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91B0BE3B-A097-4668-8A8D-B9A599E6B739}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{91B0BE3B-A097-4668-8A8D-B9A599E6B739}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>category</t>
   </si>
@@ -189,13 +189,73 @@
   </si>
   <si>
     <t>file_name</t>
+  </si>
+  <si>
+    <t>infographic</t>
+  </si>
+  <si>
+    <t>infographic1.pdf</t>
+  </si>
+  <si>
+    <t>https://support.microsoft.com/fr-fr/topic/guides-t%C3%A9l%C3%A9chargeables-6bd3eb82-0a0f-43cc-a4d2-c9f4e7ebdf39</t>
+  </si>
+  <si>
+    <t>infographic2.pdf</t>
+  </si>
+  <si>
+    <t>https://london.ca/living-london/garbage-recycling/collection-calendar</t>
+  </si>
+  <si>
+    <t>infographic3.pdf</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:ORCID_Infographic_2019.pdf</t>
+  </si>
+  <si>
+    <t>infographic4.pdf</t>
+  </si>
+  <si>
+    <t>https://www.paho.org/en/documents/infographic-pdf-hiv-prevention-2019</t>
+  </si>
+  <si>
+    <t>infographic5.pdf</t>
+  </si>
+  <si>
+    <t>https://www.heart.org/en/healthy-living/healthy-eating/add-color/seasons-of-eating-infographic</t>
+  </si>
+  <si>
+    <t>user_guide</t>
+  </si>
+  <si>
+    <t>https://cms5.revize.com/revize/cityofsedrowoolley/Departments/Solid%20Waste/CompostGuide.pdf</t>
+  </si>
+  <si>
+    <t>CompostGuide.pdf</t>
+  </si>
+  <si>
+    <t>https://download.epson-europe.com/pub/download/6296/epson629673eu.pdf</t>
+  </si>
+  <si>
+    <t>epson629673.pdf</t>
+  </si>
+  <si>
+    <t>https://data.europa.eu/sites/default/files/edp_s1_man_portal-version_4.3-user-manual_v1.0.pdf</t>
+  </si>
+  <si>
+    <t>edp_s1_man_portal-version_4.3-user-manual_v1.0.pdf</t>
+  </si>
+  <si>
+    <t>https://unfccc.int/files/national_reports/non-annex_i_national_communications/non-annex_i_inventory_software/application/pdf/naiis-user-manual.pdf</t>
+  </si>
+  <si>
+    <t>maiis-user-manual.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +267,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,15 +318,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,22 +662,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC44F0F1-E527-4C79-9711-8C371936C72F}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="38.86328125" customWidth="1"/>
     <col min="3" max="3" width="127" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +694,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -637,7 +708,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -651,7 +722,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -665,7 +736,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -679,7 +750,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -693,7 +764,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -707,7 +778,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -721,7 +792,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -735,7 +806,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -749,7 +820,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -763,7 +834,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -780,7 +851,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -797,7 +868,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -814,7 +885,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -831,7 +902,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -845,7 +916,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -859,7 +930,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -873,7 +944,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -887,7 +958,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -901,7 +972,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -915,7 +986,136 @@
         <v>45666</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="2">
+        <v>45666</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C29" r:id="rId1" xr:uid="{3B80865A-48BA-4C5B-B6F0-1A5B40358315}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(data): update docs for copyright
</commit_message>
<xml_diff>
--- a/data/pdf/metadata_pdf_file.xlsx
+++ b/data/pdf/metadata_pdf_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Wikit\Chunk_Norris\bench-chunknorris-acl2025\data\pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\Code\wikit\bench-chunknorris-acl2025\data\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61BF80-E4B1-4ACE-A3A6-E4ACA14B4851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8C3304-C3AB-45CF-B356-B4AB57ADEAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11170" xr2:uid="{91B0BE3B-A097-4668-8A8D-B9A599E6B739}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{91B0BE3B-A097-4668-8A8D-B9A599E6B739}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
   <si>
     <t>category</t>
   </si>
@@ -194,18 +194,6 @@
     <t>infographic</t>
   </si>
   <si>
-    <t>infographic1.pdf</t>
-  </si>
-  <si>
-    <t>https://support.microsoft.com/fr-fr/topic/guides-t%C3%A9l%C3%A9chargeables-6bd3eb82-0a0f-43cc-a4d2-c9f4e7ebdf39</t>
-  </si>
-  <si>
-    <t>infographic2.pdf</t>
-  </si>
-  <si>
-    <t>https://london.ca/living-london/garbage-recycling/collection-calendar</t>
-  </si>
-  <si>
     <t>infographic3.pdf</t>
   </si>
   <si>
@@ -218,12 +206,6 @@
     <t>https://www.paho.org/en/documents/infographic-pdf-hiv-prevention-2019</t>
   </si>
   <si>
-    <t>infographic5.pdf</t>
-  </si>
-  <si>
-    <t>https://www.heart.org/en/healthy-living/healthy-eating/add-color/seasons-of-eating-infographic</t>
-  </si>
-  <si>
     <t>user_guide</t>
   </si>
   <si>
@@ -233,12 +215,6 @@
     <t>CompostGuide.pdf</t>
   </si>
   <si>
-    <t>https://download.epson-europe.com/pub/download/6296/epson629673eu.pdf</t>
-  </si>
-  <si>
-    <t>epson629673.pdf</t>
-  </si>
-  <si>
     <t>https://data.europa.eu/sites/default/files/edp_s1_man_portal-version_4.3-user-manual_v1.0.pdf</t>
   </si>
   <si>
@@ -254,15 +230,9 @@
     <t>powerpoint_like</t>
   </si>
   <si>
-    <t>welcome_to_word_template.pdf</t>
-  </si>
-  <si>
     <t>microsoft_documentation</t>
   </si>
   <si>
-    <t>https://literature.rockwellautomation.com/idc/groups/literature/documents/um/test-um004_-en-p.pdf</t>
-  </si>
-  <si>
     <t>https://query.prod.cms.rt.microsoft.com/cms/api/am/binary/RE4X6Ux</t>
   </si>
   <si>
@@ -279,6 +249,18 @@
   </si>
   <si>
     <t>office-pdf.pdf</t>
+  </si>
+  <si>
+    <t>Protege5NewOWLPizzaTutorialV3.pdf</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/351037551_A_Practical_Guide_to_Building_OWL_Ontologies_Using_Protege_55_and_Plugins</t>
+  </si>
+  <si>
+    <t>6126797.pdf</t>
+  </si>
+  <si>
+    <t>https://manuals.plus/vwar/dt3-mate-sports-smart-watch-manual</t>
   </si>
 </sst>
 </file>
@@ -694,20 +676,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC44F0F1-E527-4C79-9711-8C371936C72F}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="38.796875" customWidth="1"/>
     <col min="3" max="3" width="127" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +706,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -738,7 +720,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -752,7 +734,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -766,7 +748,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -780,7 +762,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -794,7 +776,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -808,7 +790,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -822,7 +804,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -836,7 +818,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -850,7 +832,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -864,7 +846,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -881,7 +863,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -898,7 +880,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -915,7 +897,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -932,7 +914,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -946,7 +928,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -960,7 +942,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -974,7 +956,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -988,7 +970,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1002,7 +984,7 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1016,138 +998,114 @@
         <v>45666</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E24" s="2">
         <v>45666</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E25" s="2">
         <v>45666</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>60</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="2">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="2">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
       <c r="E30" s="2">
         <v>45666</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
         <v>73</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
       </c>
       <c r="C31" t="s">
         <v>74</v>
@@ -1156,46 +1114,43 @@
         <v>45667</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2">
         <v>45667</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" xr:uid="{3B80865A-48BA-4C5B-B6F0-1A5B40358315}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>